<commit_message>
Integrate yield model with TOMGRO, add monitors and version 0 of animation
</commit_message>
<xml_diff>
--- a/Hoja para calculos.xlsx
+++ b/Hoja para calculos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lili\Documents\Gama_Workspace\hydroponics\hydroponics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BD0C09F-071C-4CAF-99E1-81578A05D854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35AA2ADD-EB6A-44D9-A2A4-7B4926D359F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{9D146560-B60C-4AE1-978C-035A90D12BAE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9D146560-B60C-4AE1-978C-035A90D12BAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
   <si>
     <t>length</t>
   </si>
@@ -99,13 +99,25 @@
   </si>
   <si>
     <t>EXP 3</t>
+  </si>
+  <si>
+    <t>Solucionar error al distribuir plantas en una densidad de una planta por metro cuadrado</t>
+  </si>
+  <si>
+    <t>Animación</t>
+  </si>
+  <si>
+    <t>WIP</t>
+  </si>
+  <si>
+    <t>No esta comunicada con TOMGRO como tal es ilustrativa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,13 +125,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -134,9 +172,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -477,16 +518,16 @@
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.33203125" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="7" width="14.109375" customWidth="1"/>
+    <col min="6" max="7" width="14.140625" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>4</v>
       </c>
@@ -494,7 +535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:14" x14ac:dyDescent="0.25">
       <c r="L3" t="s">
         <v>5</v>
       </c>
@@ -503,7 +544,7 @@
         <v>0.89999999999999991</v>
       </c>
     </row>
-    <row r="4" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>0</v>
       </c>
@@ -520,7 +561,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C5">
         <f>D5*E5*I5</f>
         <v>22.499999999999996</v>
@@ -557,7 +598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>7</v>
       </c>
@@ -571,7 +612,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C10">
         <f>D10/E10/F10</f>
         <v>1.25</v>
@@ -595,15 +636,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B84ABB1F-1DE3-4F7A-A88E-552CDA920DD0}">
-  <dimension ref="B3:O19"/>
+  <dimension ref="A3:M27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="24.28515625" customWidth="1"/>
+    <col min="10" max="10" width="3.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -618,7 +663,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>7</v>
       </c>
@@ -637,7 +682,7 @@
         <v>8.6602540378443855</v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>11</v>
       </c>
@@ -649,7 +694,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F6" t="s">
         <v>14</v>
       </c>
@@ -658,7 +703,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
         <v>15</v>
       </c>
@@ -667,15 +712,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-    </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>17</v>
       </c>
@@ -695,13 +732,17 @@
         <v>19</v>
       </c>
       <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
-    </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="K13" t="s">
+        <v>17</v>
+      </c>
+      <c r="L13" t="s">
+        <v>18</v>
+      </c>
+      <c r="M13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>0</v>
       </c>
@@ -723,20 +764,27 @@
       </c>
       <c r="H14">
         <f>D14*D15*D16</f>
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="I14">
         <f>E14*E15*E16</f>
-        <v>144</v>
+        <v>12</v>
       </c>
       <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
-    </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="K14">
+        <f>C14*C15*C16</f>
+        <v>36</v>
+      </c>
+      <c r="L14">
+        <f t="shared" ref="L14:M14" si="0">D14*D15*D16</f>
+        <v>100</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>7</v>
       </c>
@@ -747,7 +795,7 @@
         <v>5</v>
       </c>
       <c r="E15">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F15" t="s">
         <v>13</v>
@@ -758,20 +806,27 @@
       </c>
       <c r="H15">
         <f>1/SQRT(D16)</f>
-        <v>0.57735026918962584</v>
+        <v>0.5</v>
       </c>
       <c r="I15">
         <f>1/SQRT(E16)</f>
+        <v>1</v>
+      </c>
+      <c r="J15" s="1"/>
+      <c r="K15">
+        <f>1/SQRT(C16)</f>
+        <v>0.57735026918962584</v>
+      </c>
+      <c r="L15">
+        <f t="shared" ref="L15:M15" si="1">1/SQRT(D16)</f>
         <v>0.5</v>
       </c>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
-    </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="M15">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>11</v>
       </c>
@@ -779,19 +834,14 @@
         <v>3</v>
       </c>
       <c r="D16">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E16">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
-    </row>
-    <row r="17" spans="6:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F17" t="s">
         <v>14</v>
       </c>
@@ -800,21 +850,28 @@
         <v>18</v>
       </c>
       <c r="H17">
-        <f t="shared" ref="H17:I17" si="0">D14*D16</f>
-        <v>15</v>
+        <f t="shared" ref="H17:I17" si="2">D14*D16</f>
+        <v>20</v>
       </c>
       <c r="I17">
-        <f t="shared" si="0"/>
-        <v>24</v>
+        <f t="shared" si="2"/>
+        <v>6</v>
       </c>
       <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="1"/>
-    </row>
-    <row r="18" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="K17">
+        <f>K14/C16</f>
+        <v>12</v>
+      </c>
+      <c r="L17">
+        <f t="shared" ref="L17:M17" si="3">L14/D16</f>
+        <v>25</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F18" t="s">
         <v>15</v>
       </c>
@@ -823,15 +880,16 @@
         <v>6</v>
       </c>
       <c r="H18">
-        <f t="shared" ref="H18:I18" si="1">D15*D16</f>
-        <v>15</v>
+        <f t="shared" ref="H18:I18" si="4">D15*D16</f>
+        <v>20</v>
       </c>
       <c r="I18">
-        <f t="shared" si="1"/>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="6:15" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F19" t="s">
         <v>16</v>
       </c>
@@ -840,13 +898,34 @@
         <v>3</v>
       </c>
       <c r="H19">
-        <f t="shared" ref="H19:I19" si="2">D16</f>
-        <v>3</v>
+        <f t="shared" ref="H19:I19" si="5">D16</f>
+        <v>4</v>
       </c>
       <c r="I19">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="J19" s="1"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D27" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -859,7 +938,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -871,7 +950,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>